<commit_message>
update logic in excel parser plugin, update import excel structure.
</commit_message>
<xml_diff>
--- a/lib/Import_file.xlsx
+++ b/lib/Import_file.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NOMP\Web\lib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="0" windowWidth="19236" windowHeight="9588"/>
+    <workbookView xWindow="4620" yWindow="0" windowWidth="19230" windowHeight="9585"/>
   </bookViews>
   <sheets>
     <sheet name="Needs" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Offers" sheetId="2" r:id="rId3"/>
     <sheet name="Actor" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Budget</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -238,6 +229,58 @@
   <si>
     <t>Marseille, France</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ticket_type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>source_actor_type</t>
+  </si>
+  <si>
+    <t>target_actor_type</t>
+  </si>
+  <si>
+    <t>contact_phone</t>
+  </si>
+  <si>
+    <t>contact_mobile</t>
+  </si>
+  <si>
+    <t>contact_email</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>creation_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>expiration_date</t>
+  </si>
+  <si>
+    <t>adresse</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -247,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +315,20 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -281,12 +338,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -298,7 +370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -311,10 +383,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -372,7 +447,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,7 +482,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +659,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,83 +669,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="17.75" customWidth="1"/>
+    <col min="11" max="11" width="13.875" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.375" customWidth="1"/>
+    <col min="14" max="14" width="16.375" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2">
         <v>33</v>
@@ -679,13 +763,13 @@
         <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="1">
         <v>41255</v>
@@ -700,27 +784,30 @@
         <v>41255</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>33</v>
@@ -729,13 +816,13 @@
         <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="1">
         <v>41255</v>
@@ -750,31 +837,30 @@
         <v>41255</v>
       </c>
       <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q3" t="e">
-        <f>+F3J3E3E3:Q3</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>33</v>
@@ -783,13 +869,13 @@
         <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="1">
         <v>41255</v>
@@ -804,10 +890,13 @@
         <v>41255</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P4" s="2">
         <v>20</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -830,126 +919,126 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -964,15 +1053,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="18.75" customWidth="1"/>
+    <col min="10" max="10" width="13.375" customWidth="1"/>
+    <col min="11" max="11" width="14.75" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="11.625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
@@ -1019,7 +1108,7 @@
         <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1123,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>